<commit_message>
First cummit with priority queue
</commit_message>
<xml_diff>
--- a/src/main/java/org/atumar4031/constants/phoneStore.xlsx
+++ b/src/main/java/org/atumar4031/constants/phoneStore.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>S/N</t>
   </si>
@@ -34,64 +34,79 @@
     <t>description</t>
   </si>
   <si>
+    <t>Nokia</t>
+  </si>
+  <si>
+    <t>charger</t>
+  </si>
+  <si>
+    <t>pin head</t>
+  </si>
+  <si>
+    <t>27vl</t>
+  </si>
+  <si>
+    <t>iphone XMas</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>16GB</t>
+  </si>
+  <si>
     <t>iphone XR</t>
   </si>
   <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>6GB</t>
+  </si>
+  <si>
+    <t>Beat soudio</t>
+  </si>
+  <si>
+    <t>headset</t>
+  </si>
+  <si>
+    <t>4GB</t>
+  </si>
+  <si>
+    <t>Kings</t>
+  </si>
+  <si>
+    <t>BT</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
     <t>iphone</t>
   </si>
   <si>
-    <t>golden</t>
-  </si>
-  <si>
-    <t>6GB</t>
-  </si>
-  <si>
-    <t>iphone XMas</t>
-  </si>
-  <si>
-    <t>white</t>
-  </si>
-  <si>
-    <t>16GB</t>
-  </si>
-  <si>
-    <t>black</t>
-  </si>
-  <si>
-    <t>iphone 7</t>
-  </si>
-  <si>
-    <t>4GB</t>
-  </si>
-  <si>
-    <t>iphone 7plus</t>
-  </si>
-  <si>
-    <t>iphone 8</t>
-  </si>
-  <si>
-    <t>Spark 7</t>
+    <t>2pace</t>
+  </si>
+  <si>
+    <t>26VL</t>
   </si>
   <si>
     <t>tecno</t>
   </si>
   <si>
-    <t>blue</t>
+    <t>24VL</t>
+  </si>
+  <si>
+    <t>Spark 5</t>
+  </si>
+  <si>
+    <t>2GB</t>
   </si>
   <si>
     <t>3GB</t>
-  </si>
-  <si>
-    <t>Spark 5</t>
-  </si>
-  <si>
-    <t>pink</t>
-  </si>
-  <si>
-    <t>2GB</t>
-  </si>
-  <si>
-    <t>Spark 4</t>
   </si>
 </sst>
 </file>
@@ -383,10 +398,10 @@
         <v>9</v>
       </c>
       <c r="E2" s="1">
-        <v>250000.0</v>
+        <v>1000.0</v>
       </c>
       <c r="F2" s="1">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>10</v>
@@ -400,10 +415,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1">
         <v>270000.0</v>
@@ -412,7 +427,7 @@
         <v>4.0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -420,13 +435,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1">
         <v>170000.0</v>
@@ -435,7 +450,7 @@
         <v>4.0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -443,13 +458,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1">
         <v>267000.0</v>
@@ -458,7 +473,7 @@
         <v>5.0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
@@ -469,10 +484,10 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1">
         <v>245000.0</v>
@@ -481,7 +496,7 @@
         <v>5.0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
@@ -489,22 +504,22 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1">
-        <v>130000.0</v>
+        <v>50000.0</v>
       </c>
       <c r="F7" s="1">
         <v>3.0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -512,22 +527,22 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1">
-        <v>245000.0</v>
+        <v>6000.0</v>
       </c>
       <c r="F8" s="1">
         <v>5.0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
@@ -535,22 +550,22 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E9" s="1">
-        <v>245000.0</v>
+        <v>12000.0</v>
       </c>
       <c r="F9" s="1">
         <v>5.0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -558,22 +573,22 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1">
-        <v>130000.0</v>
+        <v>20000.0</v>
       </c>
       <c r="F10" s="1">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
@@ -581,22 +596,22 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1">
-        <v>59000.0</v>
+        <v>2000.0</v>
       </c>
       <c r="F11" s="1">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12">
@@ -604,13 +619,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E12" s="1">
         <v>63000.0</v>
@@ -619,7 +634,7 @@
         <v>5.0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13">
@@ -627,22 +642,22 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E13" s="1">
         <v>53000.0</v>
       </c>
       <c r="F13" s="1">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>